<commit_message>
dimensions adjustment of graphs
</commit_message>
<xml_diff>
--- a/testresults1.xlsx
+++ b/testresults1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kaushallimbasiya/Documents/GitHub/CAB301-Assignment2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68A07927-D956-7443-A9DC-2BD5440AD8BC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6D98B63-BD03-4C4A-8C66-A97EE071A258}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{081349F4-0C2E-45C9-AFE0-59D10EF7212F}"/>
   </bookViews>
@@ -954,6 +954,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="7.4713980029894418E-3"/>
+              <c:y val="0.16116302931946971"/>
+            </c:manualLayout>
+          </c:layout>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3213,15 +3221,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
+      <xdr:colOff>600074</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>180974</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>190499</xdr:rowOff>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3592,7 +3600,7 @@
   <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection sqref="A1:C31"/>
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3954,7 +3962,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F96B15E3-3B8B-2941-9C5F-8182C58E2A13}">
   <dimension ref="A1:C154"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
timer tests & efficiency derivation
1 run completed for timer tests, efficiency  derivation and functionality testing
</commit_message>
<xml_diff>
--- a/testresults1.xlsx
+++ b/testresults1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10412"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kaushallimbasiya/Documents/GitHub/CAB301-Assignment2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vaibhav Vachhani\Downloads\SEM-5\CAB301\Assignment 2\Assignment2\CAB301-Assignment2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6D98B63-BD03-4C4A-8C66-A97EE071A258}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{372EDFCF-8792-496F-9B7C-D5A811DA25E7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="1" xr2:uid="{081349F4-0C2E-45C9-AFE0-59D10EF7212F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{081349F4-0C2E-45C9-AFE0-59D10EF7212F}"/>
   </bookViews>
   <sheets>
     <sheet name="testRun1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="5">
   <si>
     <t xml:space="preserve">ArraySize </t>
   </si>
@@ -45,12 +45,15 @@
   <si>
     <t>Array Size</t>
   </si>
+  <si>
+    <t>y</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -77,6 +80,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Apple bra"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -99,11 +107,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -771,6 +781,322 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-8A3A-4C93-BF91-6105CF20E096}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>testRun1!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>y</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:name>Theory comparision line</c:name>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1">
+                            <a:lumMod val="65000"/>
+                            <a:lumOff val="35000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-AU" sz="1400" baseline="0"/>
+                      <a:t>y = 2x</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-AU" sz="1400" baseline="30000"/>
+                      <a:t>2</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-AU" sz="1400"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>testRun1!$A$2:$A$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>1078</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8240</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7842</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9596</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9634</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6242</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>879</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7282</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5565</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>7689</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1625</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1187</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7124</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>9403</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1745</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3328</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>9638</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1564</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>9105</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2450</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3620</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>7139</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2520</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4151</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>9687</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>4304</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>9655</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>8845</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2851</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>4739</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>testRun1!$D$2:$D$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>2324168</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>135795200</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>122993928</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>184166432</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>185627912</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>77925128</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1545282</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>106055048</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>61938450</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>118241442</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5281250</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2817938</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>101502752</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>176832818</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6090050</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>22151168</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>185782088</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4892192</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>165802050</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>12005000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>26208800</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>101930642</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>12700800</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>34461602</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>187675938</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>37048832</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>186438050</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>156468050</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>16256402</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>44916242</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-12FB-439A-952F-73AE7D9DECF6}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1760,6 +2086,292 @@
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>testRun2!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>y</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:name>Theory comparision</c:name>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>testRun2!$A$2:$A$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>5698</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3301</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2486</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4332</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>516</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8939</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6932</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>5020</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9736</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>7913</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2175</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1273</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1372</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>682</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>9080</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5191</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>4752</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3225</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2307</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>4512</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1096</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>7685</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3940</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1374</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>3469</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>4104</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>2892</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>2477</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>8933</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>testRun2!$D$2:$D$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>64934408</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>128032002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21793202</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12360392</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>37532448</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>532512</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>159811442</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>96105248</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>50400800</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>189579392</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>125231138</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9461250</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>3241058</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3764768</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>930248</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>164892800</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>53892962</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>45163008</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>20801250</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>10644498</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>40716288</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2402432</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>118118450</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>31047200</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3775752</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>24067922</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>33685632</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>16727328</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>12271058</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>159596978</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-0580-4270-9280-7C6BF39714B8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -2034,8 +2646,8 @@
           <c:yMode val="edge"/>
           <c:x val="0.16749836758210104"/>
           <c:y val="8.0754368320782338E-2"/>
-          <c:w val="0.71980917995006721"/>
-          <c:h val="4.2572178477690285E-2"/>
+          <c:w val="0.83250167485970328"/>
+          <c:h val="4.4164875190278112E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -3597,21 +4209,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A11E0B3-0CCD-4F3C-9D7D-368DDE3E33BB}">
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.85546875" customWidth="1"/>
+    <col min="3" max="3" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="21">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3621,8 +4234,12 @@
       <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="D1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="3"/>
+    </row>
+    <row r="2" spans="1:5" ht="21">
       <c r="A2" s="3">
         <v>1078</v>
       </c>
@@ -3632,8 +4249,13 @@
       <c r="C2" s="3">
         <v>580503</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="D2" s="3">
+        <f>2*(A2*A2)</f>
+        <v>2324168</v>
+      </c>
+      <c r="E2" s="3"/>
+    </row>
+    <row r="3" spans="1:5" ht="21">
       <c r="A3" s="3">
         <v>8240</v>
       </c>
@@ -3643,8 +4265,13 @@
       <c r="C3" s="3">
         <v>33944680</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="D3" s="3">
+        <f t="shared" ref="D3:D31" si="0">2*(A3*A3)</f>
+        <v>135795200</v>
+      </c>
+      <c r="E3" s="3"/>
+    </row>
+    <row r="4" spans="1:5" ht="21">
       <c r="A4" s="3">
         <v>7842</v>
       </c>
@@ -3654,8 +4281,13 @@
       <c r="C4" s="3">
         <v>30744561</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="D4" s="3">
+        <f t="shared" si="0"/>
+        <v>122993928</v>
+      </c>
+      <c r="E4" s="3"/>
+    </row>
+    <row r="5" spans="1:5" ht="21">
       <c r="A5" s="3">
         <v>9596</v>
       </c>
@@ -3665,8 +4297,13 @@
       <c r="C5" s="3">
         <v>46036810</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="D5" s="3">
+        <f t="shared" si="0"/>
+        <v>184166432</v>
+      </c>
+      <c r="E5" s="3"/>
+    </row>
+    <row r="6" spans="1:5" ht="21">
       <c r="A6" s="3">
         <v>9634</v>
       </c>
@@ -3676,8 +4313,13 @@
       <c r="C6" s="3">
         <v>46402161</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="D6" s="3">
+        <f t="shared" si="0"/>
+        <v>185627912</v>
+      </c>
+      <c r="E6" s="3"/>
+    </row>
+    <row r="7" spans="1:5" ht="21">
       <c r="A7" s="3">
         <v>6242</v>
       </c>
@@ -3687,8 +4329,13 @@
       <c r="C7" s="3">
         <v>19478161</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="D7" s="3">
+        <f t="shared" si="0"/>
+        <v>77925128</v>
+      </c>
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" spans="1:5" ht="21">
       <c r="A8" s="3">
         <v>879</v>
       </c>
@@ -3698,8 +4345,13 @@
       <c r="C8" s="3">
         <v>385881</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="D8" s="3">
+        <f t="shared" si="0"/>
+        <v>1545282</v>
+      </c>
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" spans="1:5" ht="21">
       <c r="A9" s="3">
         <v>7282</v>
       </c>
@@ -3709,8 +4361,13 @@
       <c r="C9" s="3">
         <v>26510121</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="D9" s="3">
+        <f t="shared" si="0"/>
+        <v>106055048</v>
+      </c>
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="1:5" ht="21">
       <c r="A10" s="3">
         <v>5565</v>
       </c>
@@ -3720,8 +4377,13 @@
       <c r="C10" s="3">
         <v>15481830</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="D10" s="3">
+        <f t="shared" si="0"/>
+        <v>61938450</v>
+      </c>
+      <c r="E10" s="3"/>
+    </row>
+    <row r="11" spans="1:5" ht="21">
       <c r="A11" s="3">
         <v>7689</v>
       </c>
@@ -3731,8 +4393,13 @@
       <c r="C11" s="3">
         <v>29556516</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="D11" s="3">
+        <f t="shared" si="0"/>
+        <v>118241442</v>
+      </c>
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" spans="1:5" ht="21">
       <c r="A12" s="3">
         <v>1625</v>
       </c>
@@ -3742,8 +4409,13 @@
       <c r="C12" s="3">
         <v>1319500</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="D12" s="3">
+        <f t="shared" si="0"/>
+        <v>5281250</v>
+      </c>
+      <c r="E12" s="3"/>
+    </row>
+    <row r="13" spans="1:5" ht="21">
       <c r="A13" s="3">
         <v>1187</v>
       </c>
@@ -3753,8 +4425,13 @@
       <c r="C13" s="3">
         <v>703891</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="D13" s="3">
+        <f t="shared" si="0"/>
+        <v>2817938</v>
+      </c>
+      <c r="E13" s="3"/>
+    </row>
+    <row r="14" spans="1:5" ht="21">
       <c r="A14" s="3">
         <v>7124</v>
       </c>
@@ -3764,8 +4441,13 @@
       <c r="C14" s="3">
         <v>25372126</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="D14" s="3">
+        <f t="shared" si="0"/>
+        <v>101502752</v>
+      </c>
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" spans="1:5" ht="21">
       <c r="A15" s="3">
         <v>9403</v>
       </c>
@@ -3775,8 +4457,13 @@
       <c r="C15" s="3">
         <v>44203503</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="D15" s="3">
+        <f t="shared" si="0"/>
+        <v>176832818</v>
+      </c>
+      <c r="E15" s="3"/>
+    </row>
+    <row r="16" spans="1:5" ht="21">
       <c r="A16" s="3">
         <v>1745</v>
       </c>
@@ -3786,8 +4473,13 @@
       <c r="C16" s="3">
         <v>1521640</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="D16" s="3">
+        <f t="shared" si="0"/>
+        <v>6090050</v>
+      </c>
+      <c r="E16" s="3"/>
+    </row>
+    <row r="17" spans="1:5" ht="21">
       <c r="A17" s="3">
         <v>3328</v>
       </c>
@@ -3797,8 +4489,13 @@
       <c r="C17" s="3">
         <v>5536128</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="D17" s="3">
+        <f t="shared" si="0"/>
+        <v>22151168</v>
+      </c>
+      <c r="E17" s="3"/>
+    </row>
+    <row r="18" spans="1:5" ht="21">
       <c r="A18" s="3">
         <v>9638</v>
       </c>
@@ -3808,8 +4505,13 @@
       <c r="C18" s="3">
         <v>46440703</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="D18" s="3">
+        <f t="shared" si="0"/>
+        <v>185782088</v>
+      </c>
+      <c r="E18" s="3"/>
+    </row>
+    <row r="19" spans="1:5" ht="21">
       <c r="A19" s="3">
         <v>1564</v>
       </c>
@@ -3819,8 +4521,13 @@
       <c r="C19" s="3">
         <v>1222266</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="D19" s="3">
+        <f t="shared" si="0"/>
+        <v>4892192</v>
+      </c>
+      <c r="E19" s="3"/>
+    </row>
+    <row r="20" spans="1:5" ht="21">
       <c r="A20" s="3">
         <v>9105</v>
       </c>
@@ -3830,8 +4537,13 @@
       <c r="C20" s="3">
         <v>41445960</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="D20" s="3">
+        <f t="shared" si="0"/>
+        <v>165802050</v>
+      </c>
+      <c r="E20" s="3"/>
+    </row>
+    <row r="21" spans="1:5" ht="21">
       <c r="A21" s="3">
         <v>2450</v>
       </c>
@@ -3841,8 +4553,13 @@
       <c r="C21" s="3">
         <v>3000025</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="D21" s="3">
+        <f t="shared" si="0"/>
+        <v>12005000</v>
+      </c>
+      <c r="E21" s="3"/>
+    </row>
+    <row r="22" spans="1:5" ht="21">
       <c r="A22" s="3">
         <v>3620</v>
       </c>
@@ -3852,8 +4569,13 @@
       <c r="C22" s="3">
         <v>6550390</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="D22" s="3">
+        <f t="shared" si="0"/>
+        <v>26208800</v>
+      </c>
+      <c r="E22" s="3"/>
+    </row>
+    <row r="23" spans="1:5" ht="21">
       <c r="A23" s="3">
         <v>7139</v>
       </c>
@@ -3863,8 +4585,13 @@
       <c r="C23" s="3">
         <v>25479091</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="D23" s="3">
+        <f t="shared" si="0"/>
+        <v>101930642</v>
+      </c>
+      <c r="E23" s="3"/>
+    </row>
+    <row r="24" spans="1:5" ht="21">
       <c r="A24" s="3">
         <v>2520</v>
       </c>
@@ -3874,8 +4601,13 @@
       <c r="C24" s="3">
         <v>3173940</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="D24" s="3">
+        <f t="shared" si="0"/>
+        <v>12700800</v>
+      </c>
+      <c r="E24" s="3"/>
+    </row>
+    <row r="25" spans="1:5" ht="21">
       <c r="A25" s="3">
         <v>4151</v>
       </c>
@@ -3885,8 +4617,13 @@
       <c r="C25" s="3">
         <v>8613325</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="D25" s="3">
+        <f t="shared" si="0"/>
+        <v>34461602</v>
+      </c>
+      <c r="E25" s="3"/>
+    </row>
+    <row r="26" spans="1:5" ht="21">
       <c r="A26" s="3">
         <v>9687</v>
       </c>
@@ -3896,8 +4633,13 @@
       <c r="C26" s="3">
         <v>46914141</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="D26" s="3">
+        <f t="shared" si="0"/>
+        <v>187675938</v>
+      </c>
+      <c r="E26" s="3"/>
+    </row>
+    <row r="27" spans="1:5" ht="21">
       <c r="A27" s="3">
         <v>4304</v>
       </c>
@@ -3907,8 +4649,13 @@
       <c r="C27" s="3">
         <v>9260056</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="D27" s="3">
+        <f t="shared" si="0"/>
+        <v>37048832</v>
+      </c>
+      <c r="E27" s="3"/>
+    </row>
+    <row r="28" spans="1:5" ht="21">
       <c r="A28" s="3">
         <v>9655</v>
       </c>
@@ -3918,8 +4665,13 @@
       <c r="C28" s="3">
         <v>46604685</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="D28" s="3">
+        <f t="shared" si="0"/>
+        <v>186438050</v>
+      </c>
+      <c r="E28" s="3"/>
+    </row>
+    <row r="29" spans="1:5" ht="21">
       <c r="A29" s="3">
         <v>8845</v>
       </c>
@@ -3929,8 +4681,13 @@
       <c r="C29" s="3">
         <v>39112590</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="D29" s="3">
+        <f t="shared" si="0"/>
+        <v>156468050</v>
+      </c>
+      <c r="E29" s="3"/>
+    </row>
+    <row r="30" spans="1:5" ht="21">
       <c r="A30" s="3">
         <v>2851</v>
       </c>
@@ -3940,8 +4697,13 @@
       <c r="C30" s="3">
         <v>4062675</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="D30" s="3">
+        <f t="shared" si="0"/>
+        <v>16256402</v>
+      </c>
+      <c r="E30" s="3"/>
+    </row>
+    <row r="31" spans="1:5" ht="21">
       <c r="A31" s="3">
         <v>4739</v>
       </c>
@@ -3951,30 +4713,37 @@
       <c r="C31" s="3">
         <v>11226691</v>
       </c>
+      <c r="D31" s="3">
+        <f t="shared" si="0"/>
+        <v>44916242</v>
+      </c>
+      <c r="E31" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F96B15E3-3B8B-2941-9C5F-8182C58E2A13}">
-  <dimension ref="A1:C154"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="29.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="15.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="10.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="20.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -3984,8 +4753,11 @@
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="D1" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="20.25">
       <c r="A2" s="2">
         <v>5698</v>
       </c>
@@ -3995,8 +4767,12 @@
       <c r="C2" s="2">
         <v>16230753</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="D2" s="4">
+        <f>2*(A2*A2)</f>
+        <v>64934408</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="20.25">
       <c r="A3" s="2">
         <v>8001</v>
       </c>
@@ -4006,8 +4782,12 @@
       <c r="C3" s="2">
         <v>32004000</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="D3" s="4">
+        <f t="shared" ref="D3:D31" si="0">2*(A3*A3)</f>
+        <v>128032002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="20.25">
       <c r="A4" s="2">
         <v>3301</v>
       </c>
@@ -4017,8 +4797,12 @@
       <c r="C4" s="2">
         <v>5446650</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="D4" s="4">
+        <f t="shared" si="0"/>
+        <v>21793202</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="20.25">
       <c r="A5" s="2">
         <v>2486</v>
       </c>
@@ -4028,8 +4812,12 @@
       <c r="C5" s="2">
         <v>3088855</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="D5" s="4">
+        <f t="shared" si="0"/>
+        <v>12360392</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="20.25">
       <c r="A6" s="2">
         <v>4332</v>
       </c>
@@ -4039,8 +4827,12 @@
       <c r="C6" s="2">
         <v>9380946</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="D6" s="4">
+        <f t="shared" si="0"/>
+        <v>37532448</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="20.25">
       <c r="A7" s="2">
         <v>516</v>
       </c>
@@ -4050,8 +4842,12 @@
       <c r="C7" s="2">
         <v>132870</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="D7" s="4">
+        <f t="shared" si="0"/>
+        <v>532512</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="20.25">
       <c r="A8" s="2">
         <v>8939</v>
       </c>
@@ -4061,8 +4857,12 @@
       <c r="C8" s="2">
         <v>39948391</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="D8" s="4">
+        <f t="shared" si="0"/>
+        <v>159811442</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="20.25">
       <c r="A9" s="2">
         <v>6932</v>
       </c>
@@ -4072,8 +4872,12 @@
       <c r="C9" s="2">
         <v>24022846</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="D9" s="4">
+        <f t="shared" si="0"/>
+        <v>96105248</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="20.25">
       <c r="A10" s="2">
         <v>5020</v>
       </c>
@@ -4083,8 +4887,12 @@
       <c r="C10" s="2">
         <v>12597690</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="D10" s="4">
+        <f t="shared" si="0"/>
+        <v>50400800</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="20.25">
       <c r="A11" s="2">
         <v>9736</v>
       </c>
@@ -4094,8 +4902,12 @@
       <c r="C11" s="2">
         <v>47389980</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="D11" s="4">
+        <f t="shared" si="0"/>
+        <v>189579392</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="20.25">
       <c r="A12" s="2">
         <v>7913</v>
       </c>
@@ -4105,8 +4917,12 @@
       <c r="C12" s="2">
         <v>31303828</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="D12" s="4">
+        <f t="shared" si="0"/>
+        <v>125231138</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="20.25">
       <c r="A13" s="2">
         <v>2175</v>
       </c>
@@ -4116,8 +4932,12 @@
       <c r="C13" s="2">
         <v>2364225</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="D13" s="4">
+        <f t="shared" si="0"/>
+        <v>9461250</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="20.25">
       <c r="A14" s="2">
         <v>1273</v>
       </c>
@@ -4127,8 +4947,12 @@
       <c r="C14" s="2">
         <v>809628</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="D14" s="4">
+        <f t="shared" si="0"/>
+        <v>3241058</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="20.25">
       <c r="A15" s="2">
         <v>1372</v>
       </c>
@@ -4138,8 +4962,12 @@
       <c r="C15" s="2">
         <v>940506</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="D15" s="4">
+        <f t="shared" si="0"/>
+        <v>3764768</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="20.25">
       <c r="A16" s="2">
         <v>682</v>
       </c>
@@ -4149,8 +4977,12 @@
       <c r="C16" s="2">
         <v>232221</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="D16" s="4">
+        <f t="shared" si="0"/>
+        <v>930248</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="20.25">
       <c r="A17" s="2">
         <v>9080</v>
       </c>
@@ -4160,8 +4992,12 @@
       <c r="C17" s="2">
         <v>41218660</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="D17" s="4">
+        <f t="shared" si="0"/>
+        <v>164892800</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="20.25">
       <c r="A18" s="2">
         <v>5191</v>
       </c>
@@ -4171,8 +5007,12 @@
       <c r="C18" s="2">
         <v>13470645</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="D18" s="4">
+        <f t="shared" si="0"/>
+        <v>53892962</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="20.25">
       <c r="A19" s="2">
         <v>4752</v>
       </c>
@@ -4182,8 +5022,12 @@
       <c r="C19" s="2">
         <v>11288376</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="D19" s="4">
+        <f t="shared" si="0"/>
+        <v>45163008</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="20.25">
       <c r="A20" s="2">
         <v>3225</v>
       </c>
@@ -4193,8 +5037,12 @@
       <c r="C20" s="2">
         <v>5198700</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="D20" s="4">
+        <f t="shared" si="0"/>
+        <v>20801250</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="20.25">
       <c r="A21" s="2">
         <v>2307</v>
       </c>
@@ -4204,8 +5052,12 @@
       <c r="C21" s="2">
         <v>2659971</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="D21" s="4">
+        <f t="shared" si="0"/>
+        <v>10644498</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="20.25">
       <c r="A22" s="2">
         <v>4512</v>
       </c>
@@ -4215,8 +5067,12 @@
       <c r="C22" s="2">
         <v>10176816</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="D22" s="4">
+        <f t="shared" si="0"/>
+        <v>40716288</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="20.25">
       <c r="A23" s="2">
         <v>1096</v>
       </c>
@@ -4226,8 +5082,12 @@
       <c r="C23" s="2">
         <v>600060</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="D23" s="4">
+        <f t="shared" si="0"/>
+        <v>2402432</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="20.25">
       <c r="A24" s="2">
         <v>7685</v>
       </c>
@@ -4237,8 +5097,12 @@
       <c r="C24" s="2">
         <v>29525770</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="D24" s="4">
+        <f t="shared" si="0"/>
+        <v>118118450</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="20.25">
       <c r="A25" s="2">
         <v>3940</v>
       </c>
@@ -4248,8 +5112,12 @@
       <c r="C25" s="2">
         <v>7759830</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="D25" s="4">
+        <f t="shared" si="0"/>
+        <v>31047200</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="20.25">
       <c r="A26" s="2">
         <v>1374</v>
       </c>
@@ -4259,8 +5127,12 @@
       <c r="C26" s="2">
         <v>943251</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="D26" s="4">
+        <f t="shared" si="0"/>
+        <v>3775752</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="20.25">
       <c r="A27" s="2">
         <v>3469</v>
       </c>
@@ -4270,8 +5142,12 @@
       <c r="C27" s="2">
         <v>6015246</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="D27" s="4">
+        <f t="shared" si="0"/>
+        <v>24067922</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="20.25">
       <c r="A28" s="2">
         <v>4104</v>
       </c>
@@ -4281,8 +5157,12 @@
       <c r="C28" s="2">
         <v>8419356</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="D28" s="4">
+        <f t="shared" si="0"/>
+        <v>33685632</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="21">
       <c r="A29" s="2">
         <v>2892</v>
       </c>
@@ -4292,8 +5172,12 @@
       <c r="C29" s="2">
         <v>4180386</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="D29" s="5">
+        <f t="shared" si="0"/>
+        <v>16727328</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="21">
       <c r="A30" s="2">
         <v>2477</v>
       </c>
@@ -4303,8 +5187,12 @@
       <c r="C30" s="2">
         <v>3066526</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" s="1" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="D30" s="5">
+        <f t="shared" si="0"/>
+        <v>12271058</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="21">
       <c r="A31" s="2">
         <v>8933</v>
       </c>
@@ -4314,130 +5202,17 @@
       <c r="C31" s="2">
         <v>39894778</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="33" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="34" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="35" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="36" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="37" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="38" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="39" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="40" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="41" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="42" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="43" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="44" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="45" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="46" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="47" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="48" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="49" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="50" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="51" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="52" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="53" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="54" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="55" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="56" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="57" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="58" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="59" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="60" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="61" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="62" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="63" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="64" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="65" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="66" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="67" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="68" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="69" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="70" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="71" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="72" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="73" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="74" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="75" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="76" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="77" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="78" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="79" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="80" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="81" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="82" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="83" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="84" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="85" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="86" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="87" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="88" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="89" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="90" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="91" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="92" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="93" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="94" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="95" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="96" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="97" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="98" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="99" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="100" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="101" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="102" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="103" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="104" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="105" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="106" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="107" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="108" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="109" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="110" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="111" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="112" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="113" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="114" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="115" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="116" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="117" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="118" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="119" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="120" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="121" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="122" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="123" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="124" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="125" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="126" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="127" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="128" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="129" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="130" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="131" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="132" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="133" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="134" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="135" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="136" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="137" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="138" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="139" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="140" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="141" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="142" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="143" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="144" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="145" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="146" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="147" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="148" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="149" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="150" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="151" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="152" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="153" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="154" s="1" customFormat="1" x14ac:dyDescent="0.2"/>
+      <c r="D31" s="5">
+        <f t="shared" si="0"/>
+        <v>159596978</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="21">
+      <c r="A32" s="5"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>